<commit_message>
reparse results after fix builder
</commit_message>
<xml_diff>
--- a/results/linearincreasesizesmall10.xlsx
+++ b/results/linearincreasesizesmall10.xlsx
@@ -13,10 +13,6 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,7 +352,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G6"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,10 +362,10 @@
         <v>0.2</v>
       </c>
       <c r="B1">
-        <v>0.17280000000000001</v>
+        <v>9.6599999999999894E-2</v>
       </c>
       <c r="D1">
-        <v>5.7599999999999998E-2</v>
+        <v>2.4199999999999999E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -377,10 +373,10 @@
         <v>0.4</v>
       </c>
       <c r="B2">
-        <v>0.21579999999999999</v>
+        <v>0.105</v>
       </c>
       <c r="D2">
-        <v>8.1199999999999994E-2</v>
+        <v>3.2199999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -388,10 +384,10 @@
         <v>0.75</v>
       </c>
       <c r="B3">
-        <v>0.1762</v>
+        <v>8.8599999999999998E-2</v>
       </c>
       <c r="D3">
-        <v>7.1999999999999995E-2</v>
+        <v>2.8399999999999901E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -399,10 +395,10 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.19800000000000001</v>
+        <v>0.1094</v>
       </c>
       <c r="D4">
-        <v>6.6599999999999895E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -410,10 +406,10 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0.23100000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="D5">
-        <v>7.4800000000000005E-2</v>
+        <v>2.8399999999999901E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -421,10 +417,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.24859999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D6">
-        <v>6.0199999999999997E-2</v>
+        <v>2.21999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -432,10 +428,10 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.30839999999999901</v>
+        <v>0.22420000000000001</v>
       </c>
       <c r="D7">
-        <v>6.4199999999999993E-2</v>
+        <v>2.52E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -443,10 +439,10 @@
         <v>50</v>
       </c>
       <c r="B8">
-        <v>0.1928</v>
+        <v>0.10680000000000001</v>
       </c>
       <c r="D8">
-        <v>6.54E-2</v>
+        <v>2.5399999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,10 +450,10 @@
         <v>100</v>
       </c>
       <c r="B9">
-        <v>0.504</v>
+        <v>0.39939999999999998</v>
       </c>
       <c r="D9">
-        <v>8.4599999999999995E-2</v>
+        <v>3.2799999999999899E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -465,10 +461,10 @@
         <v>500</v>
       </c>
       <c r="B10">
-        <v>1.1221999999999901</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="D10">
-        <v>6.8599999999999994E-2</v>
+        <v>3.2399999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>